<commit_message>
add graphs, ex 2.1
</commit_message>
<xml_diff>
--- a/123/xlsx/123_pomiary_i_wykresy.xlsx
+++ b/123/xlsx/123_pomiary_i_wykresy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27900" windowHeight="12540"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27900" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kierunek przewodzenia" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>I</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>log i</t>
+  </si>
+  <si>
+    <t>Si I</t>
+  </si>
+  <si>
+    <t>świecąca I</t>
   </si>
 </sst>
 </file>
@@ -523,11 +529,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="38896768"/>
-        <c:axId val="38121856"/>
+        <c:axId val="100677504"/>
+        <c:axId val="100684160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38896768"/>
+        <c:axId val="100677504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,12 +559,17 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="38121856"/>
+        <c:spPr>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="100684160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="38121856"/>
+        <c:axId val="100684160"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -585,8 +596,8 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38896768"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="100677504"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -598,7 +609,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -615,10 +626,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11383552055993001"/>
-          <c:y val="0.18554425488480605"/>
-          <c:w val="0.72726181102362208"/>
-          <c:h val="0.65482210557013709"/>
+          <c:x val="0.11383552055993003"/>
+          <c:y val="0.18554425488480611"/>
+          <c:w val="0.7272618110236222"/>
+          <c:h val="0.6548221055701372"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -730,25 +741,25 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101984512"/>
-        <c:axId val="101297152"/>
+        <c:axId val="100991744"/>
+        <c:axId val="100993280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101984512"/>
+        <c:axId val="100991744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.30000000000000004"/>
+          <c:min val="0.3000000000000001"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="101297152"/>
+        <c:crossAx val="100993280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101297152"/>
+        <c:axId val="100993280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -757,7 +768,709 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101984512"/>
+        <c:crossAx val="100991744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dioda Ge</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$B$4:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.54</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="115109248"/>
+        <c:axId val="115107712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="115109248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115107712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="115107712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115109248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dioda Si</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$C$4:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$D$4:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="36872576"/>
+        <c:axId val="135639040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="36872576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="135639040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="135639040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="36872576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dioda świecąca</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$C$4:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$E$4:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="37454976"/>
+        <c:axId val="115143040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="37454976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115143040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="115143040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37454976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Dioda Zenera</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$G$4:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>15.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.85</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.05</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Kierunek zaporowy'!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="101053184"/>
+        <c:axId val="87569152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="101053184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="87569152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="87569152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101053184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -833,6 +1546,131 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Wykres 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1128,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1368,11 +2206,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L17:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
@@ -1409,10 +2250,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -1481,7 +2322,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E6">
-        <v>0.3</v>
+        <v>0.03</v>
       </c>
       <c r="F6">
         <v>0.3</v>
@@ -1796,6 +2637,7 @@
     <mergeCell ref="F1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix plots, add plots for kierunek zaporowy
</commit_message>
<xml_diff>
--- a/123/xlsx/123_pomiary_i_wykresy.xlsx
+++ b/123/xlsx/123_pomiary_i_wykresy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27900" windowHeight="12540" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27900" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Kierunek przewodzenia" sheetId="1" r:id="rId1"/>
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>I</t>
   </si>
   <si>
     <t>Ge</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>świecąca</t>
   </si>
   <si>
     <t>Zenera</t>
@@ -49,6 +43,18 @@
   </si>
   <si>
     <t>świecąca I</t>
+  </si>
+  <si>
+    <t>Dioda Ge</t>
+  </si>
+  <si>
+    <t>Dioda Si</t>
+  </si>
+  <si>
+    <t>Dioda świecąca</t>
+  </si>
+  <si>
+    <t>Dioda Zenera</t>
   </si>
 </sst>
 </file>
@@ -108,7 +114,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Wspólny wykres charakterystyk prądowo- napięciowych dla 4 typów diod, w skali logarytmicznej. Oznaczenie jak na rysunku.</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -122,7 +146,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ge</c:v>
+                  <c:v>Dioda Ge</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -176,42 +200,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Kierunek przewodzenia'!$A$3:$A$13</c:f>
+              <c:f>'Kierunek przewodzenia'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.69897000433601875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47712125471966244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69897000433601886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84509804001425681</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -226,7 +250,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Si</c:v>
+                  <c:v>Dioda Si</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -280,42 +304,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Kierunek przewodzenia'!$A$3:$A$13</c:f>
+              <c:f>'Kierunek przewodzenia'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.69897000433601875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47712125471966244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69897000433601886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84509804001425681</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -330,7 +354,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>świecąca</c:v>
+                  <c:v>Dioda świecąca</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -384,42 +408,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Kierunek przewodzenia'!$A$3:$A$13</c:f>
+              <c:f>'Kierunek przewodzenia'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.69897000433601875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47712125471966244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69897000433601886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84509804001425681</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -434,7 +458,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Zenera</c:v>
+                  <c:v>Dioda Zenera</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -488,52 +512,52 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Kierunek przewodzenia'!$A$3:$A$13</c:f>
+              <c:f>'Kierunek przewodzenia'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.69897000433601875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47712125471966244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69897000433601886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84509804001425681</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100677504"/>
-        <c:axId val="100684160"/>
+        <c:axId val="74424320"/>
+        <c:axId val="74426624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100677504"/>
+        <c:axId val="74424320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,14 +588,13 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="100684160"/>
+        <c:crossAx val="74426624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100684160"/>
+        <c:axId val="74426624"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -587,8 +610,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>log(I)</a:t>
+                  <a:t>log(I) [</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>µA</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -596,7 +628,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100677504"/>
+        <c:crossAx val="74424320"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -609,7 +641,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -618,20 +650,50 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
+  <c:style val="4"/>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Wykres zlinearyzowany, w skali logarytmicznej, dla diody krzemowej wraz z dopasowaną prostą.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11383552055993003"/>
-          <c:y val="0.18554425488480611"/>
-          <c:w val="0.7272618110236222"/>
-          <c:h val="0.6548221055701372"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -643,7 +705,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Si</c:v>
+                  <c:v>Dioda Si</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -654,7 +716,26 @@
             </a:ln>
           </c:spPr>
           <c:trendline>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.1323005356037828E-2"/>
+                  <c:y val="-9.5550090622626357E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </c:spPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -700,75 +781,111 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Kierunek przewodzenia'!$A$3:$A$13</c:f>
+              <c:f>'Kierunek przewodzenia'!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.69897000433601875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>-0.52287874528033762</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.3010299956639812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>-0.15490195998574319</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47712125471966244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69897000433601886</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84509804001425681</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100991744"/>
-        <c:axId val="100993280"/>
+        <c:axId val="74444160"/>
+        <c:axId val="74667520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100991744"/>
+        <c:axId val="74444160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.3000000000000001"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>U[V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="100993280"/>
+        <c:crossAx val="74667520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100993280"/>
+        <c:axId val="74667520"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1100" b="1" i="0" baseline="0"/>
+                  <a:t>log(I) [µA]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100991744"/>
+        <c:crossAx val="74444160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -792,10 +909,56 @@
   <c:lang val="pl-PL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Wykres charakterystyki  prądowo-napięciowej </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>dla </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>diody Ge</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26797462817147855"/>
+          <c:y val="2.5804397401144531E-2"/>
+        </c:manualLayout>
+      </c:layout>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11769867308253135"/>
+          <c:y val="0.3061113262481534"/>
+          <c:w val="0.67664169582968792"/>
+          <c:h val="0.49102562999297217"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -919,31 +1082,67 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="115109248"/>
-        <c:axId val="115107712"/>
+        <c:axId val="74483584"/>
+        <c:axId val="74485120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115109248"/>
+        <c:axId val="74483584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>U[V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115107712"/>
+        <c:crossAx val="74485120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115107712"/>
+        <c:axId val="74485120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1100" b="1" i="0" baseline="0"/>
+                  <a:t>log(I) [µA]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115109248"/>
+        <c:crossAx val="74483584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -956,7 +1155,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -968,6 +1167,34 @@
   <c:style val="4"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Wykres charakterystyki  prądowo- napięciowej </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>dla diody</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t> Si.</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -1095,31 +1322,69 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="36872576"/>
-        <c:axId val="135639040"/>
+        <c:axId val="74505216"/>
+        <c:axId val="74507008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36872576"/>
+        <c:axId val="74505216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>U[V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135639040"/>
+        <c:crossAx val="74507008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135639040"/>
+        <c:axId val="74507008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1100" b="1" i="0" baseline="0"/>
+                  <a:t>log(I) [µA]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36872576"/>
+        <c:crossAx val="74505216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1132,7 +1397,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1141,9 +1406,41 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
-  <c:style val="1"/>
+  <c:style val="5"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wykres charakterystyki</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>prądowo-napięciowej </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>dla diody świecącej.</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -1271,31 +1568,67 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="37454976"/>
-        <c:axId val="115143040"/>
+        <c:axId val="75071872"/>
+        <c:axId val="75073408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37454976"/>
+        <c:axId val="75071872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>U[V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115143040"/>
+        <c:crossAx val="75073408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115143040"/>
+        <c:axId val="75073408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>log(I) [µA]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37454976"/>
+        <c:crossAx val="75071872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1308,7 +1641,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1317,8 +1650,53 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
+  <c:style val="1"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wykres charakterystyki prądowo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>napięciowej </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>dla d</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>iod</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>y</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Zenera</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -1446,31 +1824,67 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101053184"/>
-        <c:axId val="87569152"/>
+        <c:axId val="75113984"/>
+        <c:axId val="75115520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101053184"/>
+        <c:axId val="75113984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>U[V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87569152"/>
+        <c:crossAx val="75115520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87569152"/>
+        <c:axId val="75115520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>log(I) [µA]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101053184"/>
+        <c:crossAx val="75113984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1483,7 +1897,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1524,19 +1938,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Wykres 9"/>
+        <xdr:cNvPr id="6" name="Wykres 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1559,15 +1973,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1588,16 +2002,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1618,16 +2032,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1648,16 +2062,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1964,17 +2378,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="12" max="12" width="9.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1985,27 +2402,27 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -2021,8 +2438,12 @@
       <c r="E3">
         <v>0.63</v>
       </c>
+      <c r="F3">
+        <f>LOG10(A3:A13)</f>
+        <v>-1</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -2038,8 +2459,12 @@
       <c r="E4">
         <v>0.65</v>
       </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F13" si="0">LOG10(A4:A14)</f>
+        <v>-0.69897000433601875</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -2055,8 +2480,12 @@
       <c r="E5">
         <v>0.67</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-0.52287874528033762</v>
+      </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>0.5</v>
       </c>
@@ -2072,8 +2501,12 @@
       <c r="E6">
         <v>0.68</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-0.3010299956639812</v>
+      </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>0.7</v>
       </c>
@@ -2089,8 +2522,12 @@
       <c r="E7">
         <v>0.7</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-0.15490195998574319</v>
+      </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2106,8 +2543,19 @@
       <c r="E8">
         <v>0.71</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="array" ref="L8:M10">LINEST(F3:F13,C3:C13,TRUE,TRUE)</f>
+        <v>10.309563332920332</v>
+      </c>
+      <c r="M8">
+        <v>-4.4869948704723432</v>
+      </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2123,8 +2571,18 @@
       <c r="E9">
         <v>0.73</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="L9">
+        <v>0.30877170215672795</v>
+      </c>
+      <c r="M9">
+        <v>0.13742942508375844</v>
+      </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2140,8 +2598,18 @@
       <c r="E10">
         <v>0.75</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="L10">
+        <v>0.99199161483193099</v>
+      </c>
+      <c r="M10">
+        <v>6.2285390020465674E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2157,8 +2625,12 @@
       <c r="E11">
         <v>0.77</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.69897000433601886</v>
+      </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>7</v>
       </c>
@@ -2174,8 +2646,12 @@
       <c r="E12">
         <v>0.79</v>
       </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.84509804001425681</v>
+      </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2190,6 +2666,10 @@
       </c>
       <c r="E13">
         <v>0.8</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2206,8 +2686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L17:L18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2221,12 +2701,12 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G1" s="2"/>
     </row>
@@ -2241,25 +2721,25 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7">

</xml_diff>